<commit_message>
Adding the rest of the content from de 1st learning path
</commit_message>
<xml_diff>
--- a/17. LinkedIn Learning/01. Microsoft Excel/01. Master Microsoft Excel - Learning Path/06. Excel - PivotTables in depth/Material/Ex_Files_Excel_Pivot_Tables_Depth/Exercise Files/Chapter02/Calculated_02_05.xlsx
+++ b/17. LinkedIn Learning/01. Microsoft Excel/01. Master Microsoft Excel - Learning Path/06. Excel - PivotTables in depth/Material/Ex_Files_Excel_Pivot_Tables_Depth/Exercise Files/Chapter02/Calculated_02_05.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Curtis\Documents\LinkedIn Learning\Excel for O365 PivotTables\Chapter02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javier García\Downloads\Excel\Learning path 01\06\Modulo 02\Ex_Files_Excel_Pivot_Tables_Depth\Ex_Files_Excel_Pivot_Tables_Depth\Exercise Files\Chapter02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B4C15D-B390-45A2-98BD-EE93E29368BF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10E20A5-B412-418C-B558-4E172658F161}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7350" xr2:uid="{2E5CF44E-A048-4B93-98D9-BFC521C6FDBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2E5CF44E-A048-4B93-98D9-BFC521C6FDBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="250">
   <si>
     <t>OrderNum</t>
   </si>
@@ -782,13 +782,16 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
     <t>Sum of Quantity</t>
+  </si>
+  <si>
+    <t>Etiquetas de fila</t>
+  </si>
+  <si>
+    <t>Suma de TotalPrice</t>
+  </si>
+  <si>
+    <t>Total general</t>
   </si>
 </sst>
 </file>
@@ -849,10 +852,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -906,7 +909,7 @@
   <cacheSource type="worksheet">
     <worksheetSource name="AllOrderDetails"/>
   </cacheSource>
-  <cacheFields count="9">
+  <cacheFields count="10">
     <cacheField name="OrderNum" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="274"/>
     </cacheField>
@@ -941,6 +944,7 @@
     <cacheField name="Unit Price" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.65" maxValue="44006"/>
     </cacheField>
+    <cacheField name="TotalPrice" numFmtId="0" formula="Quantity *'Unit Price'" databaseField="0"/>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -3971,8 +3975,8 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5AEF65CF-955B-42D9-89FE-46D9B2A545F8}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
+  <location ref="A3:C10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -3992,6 +3996,7 @@
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="4"/>
@@ -4019,11 +4024,20 @@
       <x/>
     </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
   </colItems>
-  <dataFields count="1">
+  <dataFields count="2">
     <dataField name="Sum of Quantity" fld="7" baseField="0" baseItem="0"/>
+    <dataField name="Suma de TotalPrice" fld="9" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight17" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -4059,7 +4073,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4355,80 +4369,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1265E109-71EC-4311-BAFC-2B718025FECB}">
-  <dimension ref="A3:B10"/>
+  <dimension ref="A3:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" t="s">
         <v>246</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>207</v>
       </c>
       <c r="B4" s="2">
         <v>486</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="2">
+        <v>59413232.700000018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>212</v>
       </c>
       <c r="B5" s="2">
         <v>207</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>93002202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>211</v>
       </c>
       <c r="B6" s="2">
         <v>281</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>212093.17999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>210</v>
       </c>
       <c r="B7" s="2">
         <v>739</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <v>838085.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>208</v>
       </c>
       <c r="B8" s="2">
         <v>596</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <v>18885976.479999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>209</v>
       </c>
       <c r="B9" s="2">
         <v>405</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <v>13013460</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B10" s="2">
         <v>2714</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1729480731.660002</v>
       </c>
     </row>
   </sheetData>
@@ -4444,7 +4483,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>

</xml_diff>